<commit_message>
Aggiornamento xlsx e correzione errori
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111TOPGATEXXXX/topgate/letteradimissione/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111TOPGATEXXXX/topgate/letteradimissione/1.0/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A57F84E-4BF2-47E4-B15F-09CA3C8A7CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3FA8B9-EC4F-44B3-AEE3-07233E174909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="-16200" windowWidth="14400" windowHeight="16200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="209">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -907,6 +907,9 @@
   </si>
   <si>
     <t>//</t>
+  </si>
+  <si>
+    <t>ERRORE durante la validazione &lt;risposta ricevuta dall'enpoint&gt;</t>
   </si>
 </sst>
 </file>
@@ -3811,11 +3814,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T646"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="L10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="P14" sqref="P14"/>
+      <selection pane="bottomRight" activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4375,8 +4378,8 @@
       <c r="E16" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="23" t="s">
-        <v>207</v>
+      <c r="F16" s="23">
+        <v>45072</v>
       </c>
       <c r="G16" s="24" t="s">
         <v>207</v>
@@ -4453,7 +4456,9 @@
       <c r="M17" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="N17" s="25"/>
+      <c r="N17" s="25" t="s">
+        <v>208</v>
+      </c>
       <c r="O17" s="25" t="s">
         <v>68</v>
       </c>
@@ -4505,7 +4510,9 @@
       <c r="M18" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="N18" s="25"/>
+      <c r="N18" s="25" t="s">
+        <v>208</v>
+      </c>
       <c r="O18" s="25" t="s">
         <v>68</v>
       </c>
@@ -4557,7 +4564,9 @@
       <c r="M19" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="N19" s="25"/>
+      <c r="N19" s="25" t="s">
+        <v>208</v>
+      </c>
       <c r="O19" s="25" t="s">
         <v>68</v>
       </c>
@@ -4609,7 +4618,9 @@
       <c r="M20" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="N20" s="25"/>
+      <c r="N20" s="25" t="s">
+        <v>208</v>
+      </c>
       <c r="O20" s="25" t="s">
         <v>68</v>
       </c>
@@ -4661,7 +4672,9 @@
       <c r="M21" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="N21" s="25"/>
+      <c r="N21" s="25" t="s">
+        <v>208</v>
+      </c>
       <c r="O21" s="25" t="s">
         <v>68</v>
       </c>
@@ -4713,7 +4726,9 @@
       <c r="M22" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="N22" s="25"/>
+      <c r="N22" s="25" t="s">
+        <v>208</v>
+      </c>
       <c r="O22" s="25" t="s">
         <v>68</v>
       </c>
@@ -4765,7 +4780,9 @@
       <c r="M23" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="N23" s="25"/>
+      <c r="N23" s="25" t="s">
+        <v>208</v>
+      </c>
       <c r="O23" s="25" t="s">
         <v>68</v>
       </c>
@@ -4817,7 +4834,9 @@
       <c r="M24" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="N24" s="25"/>
+      <c r="N24" s="25" t="s">
+        <v>208</v>
+      </c>
       <c r="O24" s="25" t="s">
         <v>68</v>
       </c>
@@ -4869,7 +4888,9 @@
       <c r="M25" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="N25" s="25"/>
+      <c r="N25" s="25" t="s">
+        <v>208</v>
+      </c>
       <c r="O25" s="25" t="s">
         <v>68</v>
       </c>
@@ -4921,7 +4942,9 @@
       <c r="M26" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="N26" s="25"/>
+      <c r="N26" s="25" t="s">
+        <v>208</v>
+      </c>
       <c r="O26" s="25" t="s">
         <v>68</v>
       </c>
@@ -4973,7 +4996,9 @@
       <c r="M27" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="N27" s="25"/>
+      <c r="N27" s="25" t="s">
+        <v>208</v>
+      </c>
       <c r="O27" s="25" t="s">
         <v>68</v>
       </c>
@@ -5025,7 +5050,9 @@
       <c r="M28" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="N28" s="25"/>
+      <c r="N28" s="25" t="s">
+        <v>208</v>
+      </c>
       <c r="O28" s="25" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
Correzione errori XLSX, JSON e XML
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111TOPGATEXXXX/topgate/letteradimissione/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111TOPGATEXXXX/topgate/letteradimissione/1.0/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\DA INVIARE\letteradimissione\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\FSE\DA INVIARE\letteradimissione\1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81BC21D-3D3F-4B83-9315-2482019E1E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF8CBF2-7636-4A87-B67C-0E845E6D0D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="215">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -742,18 +742,6 @@
     <t>subject_application_version: 1.0</t>
   </si>
   <si>
-    <t>2023-06-14T13:47:20+00:00</t>
-  </si>
-  <si>
-    <t>2023-06-14T13:48:04+00:00</t>
-  </si>
-  <si>
-    <t>2023-06-14T13:48:30+00:00</t>
-  </si>
-  <si>
-    <t>2023-06-14T13:48:56+00:00</t>
-  </si>
-  <si>
     <t>2023-05-26T09:49:34+00:00</t>
   </si>
   <si>
@@ -796,18 +784,6 @@
     <t>2023-05-26T10:06:49+00:00</t>
   </si>
   <si>
-    <t>54d1c55d09ed2bce</t>
-  </si>
-  <si>
-    <t>325f276f79ffbc8c</t>
-  </si>
-  <si>
-    <t>cf72cde1fcbf687e</t>
-  </si>
-  <si>
-    <t>1e387b4b40786c23</t>
-  </si>
-  <si>
     <t>2b01efa7a3930976</t>
   </si>
   <si>
@@ -847,18 +823,6 @@
     <t>2cc386a6b368dcd2</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.1cad489fa8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.0e4c168abf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.fc02628ee8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.8c27dfc679^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
@@ -908,6 +872,45 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.2560e06add^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>7622659760288830</t>
+  </si>
+  <si>
+    <t>b7ecea825b3b1b57</t>
+  </si>
+  <si>
+    <t>b4dd153c1dae76b7</t>
+  </si>
+  <si>
+    <t>2023-06-19T07:34:26+00:00</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.41724da9b7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-19T07:35:20+00:00</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.a725d805ec^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-19T08:29:20+00:00</t>
+  </si>
+  <si>
+    <t>0e48e6642d9eb7a2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.5ab8438eaf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-06-19T08:30:21+00:00</t>
+  </si>
+  <si>
+    <t>4883dcc2e199cceb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.78bac3960b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1243,7 +1246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1341,6 +1344,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3823,10 +3832,10 @@
   <dimension ref="A1:T314"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="M18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="O32" sqref="O32"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3864,12 +3873,12 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="39"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="41"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -3887,14 +3896,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="47" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="49" t="s">
         <v>155</v>
       </c>
-      <c r="D3" s="39"/>
+      <c r="D3" s="41"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -3912,12 +3921,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="47" t="s">
+      <c r="A4" s="45"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="D4" s="39"/>
+      <c r="D4" s="41"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -3936,12 +3945,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="45"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="47" t="s">
+      <c r="A5" s="47"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="D5" s="39"/>
+      <c r="D5" s="41"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -3959,8 +3968,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="36"/>
-      <c r="B6" s="37"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4015,7 +4024,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="15"/>
     </row>
-    <row r="9" spans="1:20" ht="14.25" customHeight="1">
+    <row r="9" spans="1:20" ht="14.25" customHeight="1" thickBot="1">
       <c r="A9" s="17" t="s">
         <v>24</v>
       </c>
@@ -4077,7 +4086,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="30" customHeight="1">
+    <row r="10" spans="1:20" ht="30" customHeight="1" thickBot="1">
       <c r="A10" s="20">
         <v>6</v>
       </c>
@@ -4094,16 +4103,16 @@
         <v>49</v>
       </c>
       <c r="F10" s="23">
-        <v>45091</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>193</v>
+        <v>45096</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="H10" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="I10" s="37" t="s">
+        <v>211</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>68</v>
@@ -4123,7 +4132,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="30" customHeight="1">
+    <row r="11" spans="1:20" ht="30" customHeight="1" thickBot="1">
       <c r="A11" s="20">
         <v>7</v>
       </c>
@@ -4140,16 +4149,16 @@
         <v>51</v>
       </c>
       <c r="F11" s="23">
-        <v>45091</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>194</v>
+        <v>45096</v>
+      </c>
+      <c r="G11" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="H11" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="I11" s="37" t="s">
+        <v>206</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>68</v>
@@ -4186,16 +4195,16 @@
         <v>53</v>
       </c>
       <c r="F12" s="23">
-        <v>45091</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="I12" s="24" t="s">
-        <v>195</v>
+        <v>45096</v>
+      </c>
+      <c r="G12" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="H12" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="I12" s="37" t="s">
+        <v>208</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>68</v>
@@ -4232,16 +4241,16 @@
         <v>55</v>
       </c>
       <c r="F13" s="23">
-        <v>45091</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>196</v>
+        <v>45096</v>
+      </c>
+      <c r="G13" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="H13" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="I13" s="37" t="s">
+        <v>214</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>68</v>
@@ -4281,13 +4290,13 @@
         <v>45071</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>68</v>
@@ -4335,13 +4344,13 @@
         <v>45071</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>68</v>
@@ -4389,13 +4398,13 @@
         <v>45071</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>68</v>
@@ -4445,13 +4454,13 @@
         <v>45071</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>68</v>
@@ -4499,13 +4508,13 @@
         <v>45071</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="J18" s="25" t="s">
         <v>68</v>
@@ -4553,13 +4562,13 @@
         <v>45071</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="H19" s="24">
-        <v>7622659760288830</v>
+        <v>162</v>
+      </c>
+      <c r="H19" s="36" t="s">
+        <v>202</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>68</v>
@@ -4607,13 +4616,13 @@
         <v>45071</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>68</v>
@@ -4661,13 +4670,13 @@
         <v>45071</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="H21" s="24" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>68</v>
@@ -4715,13 +4724,13 @@
         <v>45071</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="H22" s="24" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="J22" s="25" t="s">
         <v>68</v>
@@ -4769,13 +4778,13 @@
         <v>45071</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="J23" s="25" t="s">
         <v>68</v>
@@ -4823,13 +4832,13 @@
         <v>45071</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="J24" s="25" t="s">
         <v>68</v>
@@ -4877,13 +4886,13 @@
         <v>45071</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="J25" s="25" t="s">
         <v>68</v>
@@ -4931,13 +4940,13 @@
         <v>45071</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="J26" s="25" t="s">
         <v>68</v>
@@ -4985,13 +4994,13 @@
         <v>45071</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="J27" s="25" t="s">
         <v>68</v>
@@ -5039,13 +5048,13 @@
         <v>45071</v>
       </c>
       <c r="G28" s="24" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="I28" s="24" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="J28" s="25" t="s">
         <v>68</v>
@@ -5093,13 +5102,13 @@
         <v>45092</v>
       </c>
       <c r="G29" s="24" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="J29" s="25" t="s">
         <v>68</v>

</xml_diff>